<commit_message>
Add template for Google Colab
</commit_message>
<xml_diff>
--- a/templates/class2020_group00_manual.xlsx
+++ b/templates/class2020_group00_manual.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VCheplyg\Dropbox\50-tue\teaching-8QA01\8QA01 2020\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\max\OneDrive - TU Eindhoven\TUE\Sync_laptop\OGO beeldverwerking dataset\8qa01\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B2C1E2-E608-4FFE-AAA1-AEDDBBA3C6E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A5B2C1E2-E608-4FFE-AAA1-AEDDBBA3C6E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4FD6C876-9A8D-458D-B778-9B3EC68ED45F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="annotations" sheetId="1" r:id="rId1"/>
@@ -443,7 +443,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -727,9 +727,12 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -750,7 +753,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -771,7 +774,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -792,7 +795,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -813,7 +816,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -834,7 +837,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -855,7 +858,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -876,7 +879,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -897,7 +900,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -918,7 +921,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -939,7 +942,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -960,7 +963,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -981,7 +984,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1002,7 +1005,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1023,7 +1026,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1044,7 +1047,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1065,7 +1068,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1086,7 +1089,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1107,7 +1110,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1128,7 +1131,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1149,7 +1152,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1170,7 +1173,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1191,7 +1194,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1212,7 +1215,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1233,7 +1236,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1254,7 +1257,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1275,7 +1278,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1296,7 +1299,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1317,7 +1320,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1338,7 +1341,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1359,7 +1362,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1380,7 +1383,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1401,7 +1404,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1422,7 +1425,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -1443,7 +1446,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1464,7 +1467,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1485,7 +1488,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -1506,7 +1509,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1527,7 +1530,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -1548,7 +1551,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -1569,7 +1572,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -1590,7 +1593,7 @@
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -1611,7 +1614,7 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -1632,7 +1635,7 @@
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -1653,7 +1656,7 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
     </row>
-    <row r="45" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -1674,7 +1677,7 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
     </row>
-    <row r="46" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -1695,7 +1698,7 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
     </row>
-    <row r="47" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -1716,7 +1719,7 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -1737,7 +1740,7 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -1758,7 +1761,7 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -1779,7 +1782,7 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -1800,7 +1803,7 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -1821,7 +1824,7 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -1842,7 +1845,7 @@
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -1863,7 +1866,7 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
     </row>
-    <row r="55" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -1884,7 +1887,7 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
     </row>
-    <row r="56" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -1905,7 +1908,7 @@
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -1926,7 +1929,7 @@
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
     </row>
-    <row r="58" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -1947,7 +1950,7 @@
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
     </row>
-    <row r="59" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -1968,7 +1971,7 @@
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
     </row>
-    <row r="60" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -1989,7 +1992,7 @@
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
     </row>
-    <row r="61" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -2010,7 +2013,7 @@
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
     </row>
-    <row r="62" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -2031,7 +2034,7 @@
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
     </row>
-    <row r="63" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -2052,7 +2055,7 @@
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
     </row>
-    <row r="64" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -2073,7 +2076,7 @@
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
     </row>
-    <row r="65" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
@@ -2094,7 +2097,7 @@
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
     </row>
-    <row r="66" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -2115,7 +2118,7 @@
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
     </row>
-    <row r="67" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -2136,7 +2139,7 @@
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
     </row>
-    <row r="68" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -2157,7 +2160,7 @@
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
     </row>
-    <row r="69" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -2178,7 +2181,7 @@
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
     </row>
-    <row r="70" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
@@ -2199,7 +2202,7 @@
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
     </row>
-    <row r="71" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
@@ -2220,7 +2223,7 @@
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
     </row>
-    <row r="72" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
@@ -2241,7 +2244,7 @@
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
     </row>
-    <row r="73" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -2262,7 +2265,7 @@
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
     </row>
-    <row r="74" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
@@ -2283,7 +2286,7 @@
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
     </row>
-    <row r="75" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
@@ -2304,7 +2307,7 @@
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
     </row>
-    <row r="76" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
@@ -2325,7 +2328,7 @@
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
     </row>
-    <row r="77" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -2346,7 +2349,7 @@
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
     </row>
-    <row r="78" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
@@ -2367,7 +2370,7 @@
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
     </row>
-    <row r="79" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -2388,7 +2391,7 @@
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
     </row>
-    <row r="80" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
@@ -2409,7 +2412,7 @@
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
     </row>
-    <row r="81" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
@@ -2430,7 +2433,7 @@
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
     </row>
-    <row r="82" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
@@ -2451,7 +2454,7 @@
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
     </row>
-    <row r="83" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
@@ -2472,7 +2475,7 @@
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
     </row>
-    <row r="84" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
@@ -2493,7 +2496,7 @@
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
     </row>
-    <row r="85" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
@@ -2514,7 +2517,7 @@
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
     </row>
-    <row r="86" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
@@ -2535,7 +2538,7 @@
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
     </row>
-    <row r="87" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
@@ -2556,7 +2559,7 @@
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
     </row>
-    <row r="88" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
@@ -2577,7 +2580,7 @@
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
     </row>
-    <row r="89" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
@@ -2598,7 +2601,7 @@
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
     </row>
-    <row r="90" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
@@ -2619,7 +2622,7 @@
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
     </row>
-    <row r="91" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
@@ -2640,7 +2643,7 @@
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
     </row>
-    <row r="92" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
@@ -2661,7 +2664,7 @@
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
     </row>
-    <row r="93" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -2682,7 +2685,7 @@
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
     </row>
-    <row r="94" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
@@ -2703,7 +2706,7 @@
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
     </row>
-    <row r="95" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
@@ -2724,7 +2727,7 @@
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
     </row>
-    <row r="96" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
@@ -2745,7 +2748,7 @@
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
     </row>
-    <row r="97" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
@@ -2766,7 +2769,7 @@
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
     </row>
-    <row r="98" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
@@ -2787,7 +2790,7 @@
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
     </row>
-    <row r="99" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
@@ -2808,7 +2811,7 @@
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
     </row>
-    <row r="100" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
@@ -2829,7 +2832,7 @@
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
     </row>
-    <row r="101" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>114</v>
       </c>
@@ -2855,13 +2858,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>100</v>
       </c>
@@ -2869,7 +2872,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>102</v>
       </c>
@@ -2890,62 +2893,62 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>113</v>
       </c>

</xml_diff>